<commit_message>
Included support for zalenium
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata.xlsx
+++ b/src/test/resources/testdata.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="26">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -90,6 +90,9 @@
   </si>
   <si>
     <t>Validate the error message for incorrect login from SigninPageTests</t>
+  </si>
+  <si>
+    <t>No</t>
   </si>
 </sst>
 </file>
@@ -448,7 +451,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C45" sqref="C45"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -498,7 +501,7 @@
         <v>24</v>
       </c>
       <c r="C4" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>